<commit_message>
updated specification, likelihood, interventions
</commit_message>
<xml_diff>
--- a/applications/cdc_prep/Calibration Targets.xlsx
+++ b/applications/cdc_prep/Calibration Targets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruchita/Documents/Harvard/JHEEM/code/jheem_analyses/applications/cdc_prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1407508-E7F7-CC43-B1F0-08DDE55B3CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341B3ACC-B9B8-CB4B-805D-4E8C496D4F78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35800" yWindow="920" windowWidth="28040" windowHeight="17260" xr2:uid="{BCD93746-27AC-4A41-A320-991B0CDEDBA8}"/>
+    <workbookView xWindow="48420" yWindow="2020" windowWidth="19380" windowHeight="17280" xr2:uid="{BCD93746-27AC-4A41-A320-991B0CDEDBA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,10 +53,10 @@
     <t>South not reported</t>
   </si>
   <si>
-    <t>Number Eligible 2025</t>
+    <t>Louisiana</t>
   </si>
   <si>
-    <t>Louisiana</t>
+    <t>Number Eligible 2022</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A2:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,7 +582,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1">
         <v>17146</v>
@@ -603,5 +603,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>